<commit_message>
Calculod e volume da encomenda. Calculo de percentagem da encomenda. Metoso auxiliares para calculo
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -79,8 +79,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -101,7 +103,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -109,6 +111,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -116,6 +119,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -532,25 +536,29 @@
       <c r="B7" s="2">
         <v>0.94930555555555562</v>
       </c>
+      <c r="C7" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>41842</v>
+        <v>41843</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>41843</v>
+        <v>41844</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>41844</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
         <v>41845</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17">
+        <f>25*400</f>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nova classe Mapa Artigo para guardar artigos e quantidade, Alteracao dos metodos da ui e controller para usar mapa para efectuar calculoes de volumes e percentagens
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -484,6 +484,7 @@
       <c r="C2" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
@@ -495,6 +496,10 @@
       <c r="C3" s="2">
         <v>0.75</v>
       </c>
+      <c r="D3" s="2">
+        <f>C3-B3</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -517,6 +522,10 @@
       <c r="C5" s="2">
         <v>0.75</v>
       </c>
+      <c r="D5" s="2">
+        <f>C5-B5</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
@@ -528,6 +537,7 @@
       <c r="C6" s="2">
         <v>0.10416666666666667</v>
       </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -544,16 +554,18 @@
       <c r="A8" s="1">
         <v>41843</v>
       </c>
+      <c r="B8" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>41844</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>41845</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="17" spans="6:6">
       <c r="F17">

</xml_diff>

<commit_message>
Correcoes para o caso de uso 1(alteracoes do nome das classes). Adicao de tipo de palete e calculo de volume de encomenda com palete
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="400" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="380" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,16 @@
     <t>Hora Fim</t>
   </si>
   <si>
-    <t>Total Horas Diarias</t>
+    <t xml:space="preserve">Total Horas Diarias  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -79,7 +82,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -97,13 +100,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -112,6 +120,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -120,6 +130,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -484,7 +496,10 @@
       <c r="C2" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2" si="0">+C2-B2</f>
+        <v>-0.875</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
@@ -496,8 +511,8 @@
       <c r="C3" s="2">
         <v>0.75</v>
       </c>
-      <c r="D3" s="2">
-        <f>C3-B3</f>
+      <c r="D3" s="3">
+        <f>+C3-B3</f>
         <v>0.125</v>
       </c>
     </row>
@@ -511,6 +526,10 @@
       <c r="C4" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D11" si="1">+C4-B4</f>
+        <v>-0.875</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
@@ -522,8 +541,8 @@
       <c r="C5" s="2">
         <v>0.75</v>
       </c>
-      <c r="D5" s="2">
-        <f>C5-B5</f>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
     </row>
@@ -537,7 +556,10 @@
       <c r="C6" s="2">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.8125</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -549,6 +571,10 @@
       <c r="C7" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="D7" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.90763888888888899</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
@@ -560,17 +586,54 @@
       <c r="C8" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.89583333333333337</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>41845</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C9" s="2">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.86111111111111116</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="17" spans="6:6">
-      <c r="F17">
-        <f>25*400</f>
-        <v>10000</v>
+      <c r="A10" s="1">
+        <v>41846</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.14583333333333337</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>41849</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.91666666666666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>